<commit_message>
Fix v1.6A Screw Terminals
Make part number correct and no substitute
</commit_message>
<xml_diff>
--- a/Source/Outputs/V3D_RUMBA_v1_6A_BOM.xlsx
+++ b/Source/Outputs/V3D_RUMBA_v1_6A_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PCB Design\A3D - RUMBA\RUMBA-Plus\Source\Outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{90F5466B-C029-4D33-B35E-D7577F86D7D9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE2F9781-62E8-46EB-9BFC-5847E0475A99}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32310" yWindow="3510" windowWidth="21600" windowHeight="12735" xr2:uid="{8783A3D6-F1A3-4A2A-BDFC-E286EEF94DF1}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="12735" xr2:uid="{9FDE391C-EA9B-4578-B35F-79AE4A654EEB}"/>
   </bookViews>
   <sheets>
     <sheet name="V3D_RUMBA_v1_6A_BOM" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="157">
   <si>
     <t>Designator</t>
   </si>
@@ -459,13 +459,16 @@
     <t>TERM BLK 2POS SIDE ENT 3.5MM PCB</t>
   </si>
   <si>
-    <t>Phoenix Contact</t>
-  </si>
-  <si>
-    <t>1751248</t>
-  </si>
-  <si>
-    <t>277-5719-ND</t>
+    <t/>
+  </si>
+  <si>
+    <t>TE Connectivity</t>
+  </si>
+  <si>
+    <t>284391/2</t>
+  </si>
+  <si>
+    <t>A98159-ND</t>
   </si>
   <si>
     <t>HB-OUT, HB-PWR, MAIN-PWR</t>
@@ -474,10 +477,10 @@
     <t>TERM BLK 2POS SIDE ENTRY 5MM PCB</t>
   </si>
   <si>
-    <t>1935776</t>
-  </si>
-  <si>
-    <t>277-6405-ND</t>
+    <t>282856-2</t>
+  </si>
+  <si>
+    <t>A98355-ND</t>
   </si>
   <si>
     <t>E0_MOT, E1_MOT, E2_MOT, X_MOT, Y_MOT, Z_MOT</t>
@@ -486,10 +489,10 @@
     <t>TERM BLK 4POS SIDE ENT 3.5MM PCB</t>
   </si>
   <si>
-    <t>1751264</t>
-  </si>
-  <si>
-    <t>277-5744-ND</t>
+    <t>284391-4</t>
+  </si>
+  <si>
+    <t>A98161-ND</t>
   </si>
   <si>
     <t>U5</t>
@@ -886,7 +889,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6261F5D-3BD3-41C8-9E68-1F4FFBD7E619}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55090EAB-B756-4612-BA2C-027E5B5B4580}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -1703,79 +1706,79 @@
         <v>5</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>10</v>
+        <v>140</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G33" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C34" s="4">
         <v>3</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>10</v>
+        <v>140</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G34" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C35" s="4">
         <v>6</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>10</v>
+        <v>140</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G35" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C36" s="4">
         <v>1</v>
@@ -1784,16 +1787,16 @@
         <v>10</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="G36" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>